<commit_message>
Update .csv and .json after october migration (#106)
* fixing columns order and regenerating
* update export table
* regenerating xlsx

---------

Co-authored-by: Monnerat Marc swisstopo <marc.monnerat@swisstopo.ch>
</commit_message>
<xml_diff>
--- a/exports/export_tables.xlsx
+++ b/exports/export_tables.xlsx
@@ -11,10 +11,9 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="LITHO" sheetId="2" state="visible" r:id="rId2"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="LITSTRAT" sheetId="3" state="visible" r:id="rId3"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TECTO" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SYSTEM" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="COMPOSIT" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ADMIXTURE" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="CHARCAT" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="COMPOSIT" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ADMIXTURE" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="CHARCAT" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -92638,407 +92637,6 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>OBJECTID</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>GEOL_CODE_INT</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>GEOL_CODE</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>GERMAN</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" t="n">
-        <v>12903001</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Lfos103001</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Vertebraten</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="n">
-        <v>12903002</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Lfos103002</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Ostrakoden</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="n">
-        <v>12903003</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Lfos103003</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Gastropoden</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="n">
-        <v>12903004</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Lfos103004</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Foraminiferen</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="n">
-        <v>12903005</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Lfos103005</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Algen</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="n">
-        <v>12903006</v>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Lfos103006</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Blätter</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" t="n">
-        <v>12903007</v>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Lfos103007</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Gräser</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" t="n">
-        <v>12903008</v>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Lfos103008</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>Holz</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" t="n">
-        <v>12903009</v>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Lfos103009</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Ammoniten</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" t="n">
-        <v>12903010</v>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Lfos103010</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Schwämme</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="B12" t="n">
-        <v>12903011</v>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Lfos103011</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>Korallen</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="B13" t="n">
-        <v>12903012</v>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Lfos103012</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>Brachiopoden</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="B14" t="n">
-        <v>12903013</v>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Lfos103013</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>Mollusken</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="B15" t="n">
-        <v>12903014</v>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>Lfos103014</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>Cephalopoden</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="B16" t="n">
-        <v>12903015</v>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>Lfos103015</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>Bivalven</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="B17" t="n">
-        <v>12903016</v>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>Lfos103016</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>Echinodermen</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="B18" t="n">
-        <v>12903017</v>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>Lfos103017</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>Fische</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="B19" t="n">
-        <v>12903018</v>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>Lfos103018</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>Reptilien</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="B20" t="n">
-        <v>12903019</v>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>Lfos103019</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>Säugetiere</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="B21" t="n">
-        <v>12903021</v>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>Lfos103021</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>Palynomorphe</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -93200,7 +92798,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -93475,7 +93073,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>